<commit_message>
topsis works with id
</commit_message>
<xml_diff>
--- a/SWD_baza_danych.xlsx
+++ b/SWD_baza_danych.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27316"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27318"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aghedupl-my.sharepoint.com/personal/stecb_student_agh_edu_pl/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3CD2BAEC-5C0D-49F8-A348-0282A6BE17B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD8277C6-E521-44CA-9652-5D030B1D3D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E7BD0E20-36F2-4D6E-9FAD-2A8832F565CC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Cena [zł]</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>balkon</t>
+  </si>
+  <si>
+    <t>id mieszkania</t>
   </si>
 </sst>
 </file>
@@ -417,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC590367-7954-4AF8-B792-655F594540BA}">
-  <dimension ref="A1:G258"/>
+  <dimension ref="A1:H258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" topLeftCell="A246" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -435,7 +438,7 @@
     <col min="8" max="8" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15">
+    <row r="1" spans="1:8" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -457,8 +460,11 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15">
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15">
       <c r="A2" s="1">
         <v>799000</v>
       </c>
@@ -480,8 +486,11 @@
       <c r="G2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15">
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15">
       <c r="A3" s="1">
         <v>299000</v>
       </c>
@@ -503,8 +512,11 @@
       <c r="G3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15">
+      <c r="H3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15">
       <c r="A4" s="1">
         <v>640000</v>
       </c>
@@ -526,8 +538,11 @@
       <c r="G4" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15">
+      <c r="H4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15">
       <c r="A5" s="1">
         <v>1418500</v>
       </c>
@@ -549,8 +564,11 @@
       <c r="G5" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15">
+      <c r="H5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15">
       <c r="A6" s="1">
         <v>1050000</v>
       </c>
@@ -572,8 +590,11 @@
       <c r="G6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="15">
+      <c r="H6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15">
       <c r="A7" s="1">
         <v>182400</v>
       </c>
@@ -595,8 +616,11 @@
       <c r="G7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="15">
+      <c r="H7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15">
       <c r="A8" s="1">
         <v>780000</v>
       </c>
@@ -618,8 +642,11 @@
       <c r="G8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="15">
+      <c r="H8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15">
       <c r="A9" s="1">
         <v>1199000</v>
       </c>
@@ -641,8 +668,11 @@
       <c r="G9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15">
+      <c r="H9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15">
       <c r="A10" s="1">
         <v>169000</v>
       </c>
@@ -664,8 +694,11 @@
       <c r="G10" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15">
+      <c r="H10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15">
       <c r="A11" s="1">
         <v>1097000</v>
       </c>
@@ -687,8 +720,11 @@
       <c r="G11" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="15">
+      <c r="H11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15">
       <c r="A12" s="1">
         <v>775000</v>
       </c>
@@ -710,8 +746,11 @@
       <c r="G12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="15">
+      <c r="H12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15">
       <c r="A13" s="1">
         <v>620000</v>
       </c>
@@ -733,8 +772,11 @@
       <c r="G13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="15">
+      <c r="H13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15">
       <c r="A14" s="1">
         <v>760000</v>
       </c>
@@ -756,8 +798,11 @@
       <c r="G14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="15">
+      <c r="H14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15">
       <c r="A15" s="1">
         <v>1050000</v>
       </c>
@@ -779,8 +824,11 @@
       <c r="G15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="15">
+      <c r="H15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15">
       <c r="A16" s="1">
         <v>535000</v>
       </c>
@@ -802,8 +850,11 @@
       <c r="G16" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="15">
+      <c r="H16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15">
       <c r="A17" s="1">
         <v>1185000</v>
       </c>
@@ -825,8 +876,11 @@
       <c r="G17" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="15">
+      <c r="H17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15">
       <c r="A18" s="1">
         <v>1548000</v>
       </c>
@@ -848,8 +902,11 @@
       <c r="G18" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="15">
+      <c r="H18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15">
       <c r="A19" s="1">
         <v>774148</v>
       </c>
@@ -871,8 +928,11 @@
       <c r="G19" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="15">
+      <c r="H19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15">
       <c r="A20" s="1">
         <v>669000</v>
       </c>
@@ -894,8 +954,11 @@
       <c r="G20" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="15">
+      <c r="H20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15">
       <c r="A21" s="1">
         <v>2100000</v>
       </c>
@@ -917,8 +980,11 @@
       <c r="G21" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="15">
+      <c r="H21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15">
       <c r="A22" s="1">
         <v>1026000</v>
       </c>
@@ -940,8 +1006,11 @@
       <c r="G22" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="15">
+      <c r="H22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15">
       <c r="A23" s="1">
         <v>1847000</v>
       </c>
@@ -963,8 +1032,11 @@
       <c r="G23" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="15">
+      <c r="H23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15">
       <c r="A24" s="1">
         <v>2039000</v>
       </c>
@@ -986,8 +1058,11 @@
       <c r="G24" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="15">
+      <c r="H24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15">
       <c r="A25" s="1">
         <v>1861000</v>
       </c>
@@ -1009,8 +1084,11 @@
       <c r="G25" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="15">
+      <c r="H25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15">
       <c r="A26" s="1">
         <v>715000</v>
       </c>
@@ -1032,8 +1110,11 @@
       <c r="G26" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="15">
+      <c r="H26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15">
       <c r="A27" s="1">
         <v>1219000</v>
       </c>
@@ -1055,8 +1136,11 @@
       <c r="G27" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="15">
+      <c r="H27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15">
       <c r="A28" s="1">
         <v>1125000</v>
       </c>
@@ -1078,8 +1162,11 @@
       <c r="G28" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="15">
+      <c r="H28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15">
       <c r="A29" s="1">
         <v>1127000</v>
       </c>
@@ -1101,8 +1188,11 @@
       <c r="G29" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="15">
+      <c r="H29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15">
       <c r="A30" s="1">
         <v>943000</v>
       </c>
@@ -1124,8 +1214,11 @@
       <c r="G30" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="15">
+      <c r="H30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15">
       <c r="A31" s="1">
         <v>888000</v>
       </c>
@@ -1147,8 +1240,11 @@
       <c r="G31" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="15">
+      <c r="H31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15">
       <c r="A32" s="1">
         <v>1954000</v>
       </c>
@@ -1170,8 +1266,11 @@
       <c r="G32" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="15">
+      <c r="H32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15">
       <c r="A33" s="1">
         <v>387000</v>
       </c>
@@ -1193,8 +1292,11 @@
       <c r="G33" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="15">
+      <c r="H33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15">
       <c r="A34" s="1">
         <v>1893000</v>
       </c>
@@ -1216,8 +1318,11 @@
       <c r="G34" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="15">
+      <c r="H34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15">
       <c r="A35" s="1">
         <v>945000</v>
       </c>
@@ -1239,8 +1344,11 @@
       <c r="G35" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="15">
+      <c r="H35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15">
       <c r="A36" s="1">
         <v>1226000</v>
       </c>
@@ -1262,8 +1370,11 @@
       <c r="G36" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="15">
+      <c r="H36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15">
       <c r="A37" s="1">
         <v>1980000</v>
       </c>
@@ -1285,8 +1396,11 @@
       <c r="G37" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="15">
+      <c r="H37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15">
       <c r="A38" s="1">
         <v>465000</v>
       </c>
@@ -1308,8 +1422,11 @@
       <c r="G38" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="15">
+      <c r="H38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15">
       <c r="A39" s="1">
         <v>1112000</v>
       </c>
@@ -1331,8 +1448,11 @@
       <c r="G39" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="15">
+      <c r="H39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15">
       <c r="A40" s="1">
         <v>1566000</v>
       </c>
@@ -1354,8 +1474,11 @@
       <c r="G40" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="15">
+      <c r="H40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15">
       <c r="A41" s="1">
         <v>686000</v>
       </c>
@@ -1377,8 +1500,11 @@
       <c r="G41" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" ht="15">
+      <c r="H41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15">
       <c r="A42" s="1">
         <v>584000</v>
       </c>
@@ -1400,8 +1526,11 @@
       <c r="G42" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="15">
+      <c r="H42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15">
       <c r="A43" s="1">
         <v>1750000</v>
       </c>
@@ -1423,8 +1552,11 @@
       <c r="G43" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="15">
+      <c r="H43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15">
       <c r="A44" s="1">
         <v>1325000</v>
       </c>
@@ -1446,8 +1578,11 @@
       <c r="G44" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" ht="15">
+      <c r="H44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15">
       <c r="A45" s="1">
         <v>915000</v>
       </c>
@@ -1469,8 +1604,11 @@
       <c r="G45" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" ht="15">
+      <c r="H45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15">
       <c r="A46" s="1">
         <v>471000</v>
       </c>
@@ -1492,8 +1630,11 @@
       <c r="G46" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" ht="15">
+      <c r="H46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15">
       <c r="A47" s="1">
         <v>923000</v>
       </c>
@@ -1515,8 +1656,11 @@
       <c r="G47" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" ht="15">
+      <c r="H47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15">
       <c r="A48" s="1">
         <v>461000</v>
       </c>
@@ -1538,8 +1682,11 @@
       <c r="G48" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" ht="15">
+      <c r="H48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15">
       <c r="A49" s="1">
         <v>1056000</v>
       </c>
@@ -1561,8 +1708,11 @@
       <c r="G49" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" ht="15">
+      <c r="H49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15">
       <c r="A50" s="1">
         <v>1209000</v>
       </c>
@@ -1584,8 +1734,11 @@
       <c r="G50" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" ht="15">
+      <c r="H50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="15">
       <c r="A51" s="1">
         <v>1824000</v>
       </c>
@@ -1607,8 +1760,11 @@
       <c r="G51" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" ht="15">
+      <c r="H51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="15">
       <c r="A52" s="1">
         <v>1602000</v>
       </c>
@@ -1630,8 +1786,11 @@
       <c r="G52" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" ht="15">
+      <c r="H52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="15">
       <c r="A53" s="1">
         <v>1341000</v>
       </c>
@@ -1653,8 +1812,11 @@
       <c r="G53" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" ht="15">
+      <c r="H53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="15">
       <c r="A54" s="1">
         <v>425000</v>
       </c>
@@ -1676,8 +1838,11 @@
       <c r="G54" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" ht="15">
+      <c r="H54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="15">
       <c r="A55" s="1">
         <v>1966000</v>
       </c>
@@ -1699,8 +1864,11 @@
       <c r="G55" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" ht="15">
+      <c r="H55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="15">
       <c r="A56" s="1">
         <v>537000</v>
       </c>
@@ -1722,8 +1890,11 @@
       <c r="G56" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" ht="15">
+      <c r="H56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="15">
       <c r="A57" s="1">
         <v>835000</v>
       </c>
@@ -1745,8 +1916,11 @@
       <c r="G57" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" ht="15">
+      <c r="H57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="15">
       <c r="A58" s="1">
         <v>1050000</v>
       </c>
@@ -1768,8 +1942,11 @@
       <c r="G58" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" ht="15">
+      <c r="H58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="15">
       <c r="A59" s="1">
         <v>422000</v>
       </c>
@@ -1791,8 +1968,11 @@
       <c r="G59" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" ht="15">
+      <c r="H59">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="15">
       <c r="A60" s="1">
         <v>387000</v>
       </c>
@@ -1814,8 +1994,11 @@
       <c r="G60" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" ht="15">
+      <c r="H60">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="15">
       <c r="A61" s="1">
         <v>218000</v>
       </c>
@@ -1837,8 +2020,11 @@
       <c r="G61" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" ht="15">
+      <c r="H61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="15">
       <c r="A62" s="1">
         <v>258000</v>
       </c>
@@ -1860,8 +2046,11 @@
       <c r="G62" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" ht="15">
+      <c r="H62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="15">
       <c r="A63" s="1">
         <v>1651000</v>
       </c>
@@ -1883,8 +2072,11 @@
       <c r="G63" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" ht="15">
+      <c r="H63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="15">
       <c r="A64" s="1">
         <v>392000</v>
       </c>
@@ -1906,8 +2098,11 @@
       <c r="G64" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" ht="15">
+      <c r="H64">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="15">
       <c r="A65" s="1">
         <v>943000</v>
       </c>
@@ -1929,8 +2124,11 @@
       <c r="G65" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" ht="15">
+      <c r="H65">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="15">
       <c r="A66" s="1">
         <v>1556000</v>
       </c>
@@ -1952,8 +2150,11 @@
       <c r="G66" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" ht="15">
+      <c r="H66">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="15">
       <c r="A67" s="1">
         <v>966000</v>
       </c>
@@ -1975,8 +2176,11 @@
       <c r="G67" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" ht="15">
+      <c r="H67">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="15">
       <c r="A68" s="1">
         <v>196000</v>
       </c>
@@ -1998,8 +2202,11 @@
       <c r="G68" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" ht="15">
+      <c r="H68">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="15">
       <c r="A69" s="1">
         <v>228000</v>
       </c>
@@ -2021,8 +2228,11 @@
       <c r="G69" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" ht="15">
+      <c r="H69">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="15">
       <c r="A70" s="1">
         <v>1442000</v>
       </c>
@@ -2044,8 +2254,11 @@
       <c r="G70" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" ht="15">
+      <c r="H70">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="15">
       <c r="A71" s="1">
         <v>1908000</v>
       </c>
@@ -2067,8 +2280,11 @@
       <c r="G71" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" ht="15">
+      <c r="H71">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="15">
       <c r="A72" s="1">
         <v>1324000</v>
       </c>
@@ -2090,8 +2306,11 @@
       <c r="G72" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" ht="15">
+      <c r="H72">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="15">
       <c r="A73" s="1">
         <v>1463000</v>
       </c>
@@ -2113,8 +2332,11 @@
       <c r="G73" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" ht="15">
+      <c r="H73">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="15">
       <c r="A74" s="1">
         <v>1095000</v>
       </c>
@@ -2136,8 +2358,11 @@
       <c r="G74" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" ht="15">
+      <c r="H74">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="15">
       <c r="A75" s="1">
         <v>1689000</v>
       </c>
@@ -2159,8 +2384,11 @@
       <c r="G75" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" ht="15">
+      <c r="H75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="15">
       <c r="A76" s="1">
         <v>472000</v>
       </c>
@@ -2182,8 +2410,11 @@
       <c r="G76" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" ht="15">
+      <c r="H76">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="15">
       <c r="A77" s="1">
         <v>662000</v>
       </c>
@@ -2205,8 +2436,11 @@
       <c r="G77" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" ht="15">
+      <c r="H77">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="15">
       <c r="A78" s="1">
         <v>1101000</v>
       </c>
@@ -2228,8 +2462,11 @@
       <c r="G78" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" ht="15">
+      <c r="H78">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="15">
       <c r="A79" s="1">
         <v>1691000</v>
       </c>
@@ -2251,8 +2488,11 @@
       <c r="G79" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" ht="15">
+      <c r="H79">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="15">
       <c r="A80" s="1">
         <v>1112000</v>
       </c>
@@ -2274,8 +2514,11 @@
       <c r="G80" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" ht="15">
+      <c r="H80">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="15">
       <c r="A81" s="1">
         <v>236000</v>
       </c>
@@ -2297,8 +2540,11 @@
       <c r="G81" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" ht="15">
+      <c r="H81">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="15">
       <c r="A82" s="1">
         <v>1859000</v>
       </c>
@@ -2320,8 +2566,11 @@
       <c r="G82" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" ht="15">
+      <c r="H82">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="15">
       <c r="A83" s="1">
         <v>1185000</v>
       </c>
@@ -2343,8 +2592,11 @@
       <c r="G83" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" ht="15">
+      <c r="H83">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="15">
       <c r="A84" s="1">
         <v>1942000</v>
       </c>
@@ -2366,8 +2618,11 @@
       <c r="G84" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" ht="15">
+      <c r="H84">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="15">
       <c r="A85" s="1">
         <v>1440000</v>
       </c>
@@ -2389,8 +2644,11 @@
       <c r="G85" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" ht="15">
+      <c r="H85">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="15">
       <c r="A86" s="1">
         <v>875000</v>
       </c>
@@ -2412,8 +2670,11 @@
       <c r="G86" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" ht="15">
+      <c r="H86">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="15">
       <c r="A87" s="1">
         <v>932000</v>
       </c>
@@ -2435,8 +2696,11 @@
       <c r="G87" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" ht="15">
+      <c r="H87">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="15">
       <c r="A88" s="1">
         <v>1388000</v>
       </c>
@@ -2458,8 +2722,11 @@
       <c r="G88" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" ht="15">
+      <c r="H88">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="15">
       <c r="A89" s="1">
         <v>1023000</v>
       </c>
@@ -2481,8 +2748,11 @@
       <c r="G89" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" ht="15">
+      <c r="H89">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="15">
       <c r="A90" s="1">
         <v>1973000</v>
       </c>
@@ -2504,8 +2774,11 @@
       <c r="G90" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" ht="15">
+      <c r="H90">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="15">
       <c r="A91" s="1">
         <v>1058000</v>
       </c>
@@ -2527,8 +2800,11 @@
       <c r="G91" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" ht="15">
+      <c r="H91">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="15">
       <c r="A92" s="1">
         <v>871000</v>
       </c>
@@ -2550,8 +2826,11 @@
       <c r="G92" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" ht="15">
+      <c r="H92">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="15">
       <c r="A93" s="1">
         <v>569000</v>
       </c>
@@ -2573,8 +2852,11 @@
       <c r="G93" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" ht="15">
+      <c r="H93">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="15">
       <c r="A94" s="1">
         <v>1563000</v>
       </c>
@@ -2596,8 +2878,11 @@
       <c r="G94" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" ht="15">
+      <c r="H94">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="15">
       <c r="A95" s="1">
         <v>1389000</v>
       </c>
@@ -2619,8 +2904,11 @@
       <c r="G95" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" ht="15">
+      <c r="H95">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="15">
       <c r="A96" s="1">
         <v>1021000</v>
       </c>
@@ -2642,8 +2930,11 @@
       <c r="G96" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" ht="15">
+      <c r="H96">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="15">
       <c r="A97" s="1">
         <v>925000</v>
       </c>
@@ -2665,8 +2956,11 @@
       <c r="G97" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" ht="15">
+      <c r="H97">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="15">
       <c r="A98" s="1">
         <v>934000</v>
       </c>
@@ -2688,8 +2982,11 @@
       <c r="G98" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" ht="15">
+      <c r="H98">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="15">
       <c r="A99" s="1">
         <v>1661000</v>
       </c>
@@ -2711,8 +3008,11 @@
       <c r="G99" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" ht="15">
+      <c r="H99">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="15">
       <c r="A100" s="1">
         <v>648000</v>
       </c>
@@ -2734,8 +3034,11 @@
       <c r="G100" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" ht="15">
+      <c r="H100">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="15">
       <c r="A101" s="1">
         <v>438000</v>
       </c>
@@ -2757,8 +3060,11 @@
       <c r="G101" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" ht="15">
+      <c r="H101">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="15">
       <c r="A102" s="1">
         <v>645000</v>
       </c>
@@ -2780,8 +3086,11 @@
       <c r="G102" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" ht="15">
+      <c r="H102">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="15">
       <c r="A103" s="1">
         <v>1923000</v>
       </c>
@@ -2803,8 +3112,11 @@
       <c r="G103" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" ht="15">
+      <c r="H103">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="15">
       <c r="A104" s="1">
         <v>1937000</v>
       </c>
@@ -2826,8 +3138,11 @@
       <c r="G104" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" ht="15">
+      <c r="H104">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="15">
       <c r="A105" s="1">
         <v>459000</v>
       </c>
@@ -2849,8 +3164,11 @@
       <c r="G105" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" ht="15">
+      <c r="H105">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="15">
       <c r="A106" s="1">
         <v>597000</v>
       </c>
@@ -2872,8 +3190,11 @@
       <c r="G106" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" ht="15">
+      <c r="H106">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="15">
       <c r="A107" s="1">
         <v>558000</v>
       </c>
@@ -2895,8 +3216,11 @@
       <c r="G107" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" ht="15">
+      <c r="H107">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="15">
       <c r="A108" s="1">
         <v>1734000</v>
       </c>
@@ -2918,8 +3242,11 @@
       <c r="G108" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" ht="15">
+      <c r="H108">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="15">
       <c r="A109" s="1">
         <v>544000</v>
       </c>
@@ -2941,8 +3268,11 @@
       <c r="G109" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" ht="15">
+      <c r="H109">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="15">
       <c r="A110" s="1">
         <v>839000</v>
       </c>
@@ -2964,8 +3294,11 @@
       <c r="G110" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" ht="15">
+      <c r="H110">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="15">
       <c r="A111" s="1">
         <v>1238000</v>
       </c>
@@ -2987,8 +3320,11 @@
       <c r="G111" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" ht="15">
+      <c r="H111">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="15">
       <c r="A112" s="1">
         <v>1790000</v>
       </c>
@@ -3010,8 +3346,11 @@
       <c r="G112" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" ht="15">
+      <c r="H112">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="15">
       <c r="A113" s="1">
         <v>245000</v>
       </c>
@@ -3033,8 +3372,11 @@
       <c r="G113" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" ht="15">
+      <c r="H113">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="15">
       <c r="A114" s="1">
         <v>315000</v>
       </c>
@@ -3056,8 +3398,11 @@
       <c r="G114" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" ht="15">
+      <c r="H114">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="15">
       <c r="A115" s="1">
         <v>989000</v>
       </c>
@@ -3079,8 +3424,11 @@
       <c r="G115" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" ht="15">
+      <c r="H115">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="15">
       <c r="A116" s="1">
         <v>899000</v>
       </c>
@@ -3102,8 +3450,11 @@
       <c r="G116" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" ht="15">
+      <c r="H116">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="15">
       <c r="A117" s="1">
         <v>742000</v>
       </c>
@@ -3125,8 +3476,11 @@
       <c r="G117" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" ht="15">
+      <c r="H117">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="15">
       <c r="A118" s="1">
         <v>712000</v>
       </c>
@@ -3148,8 +3502,11 @@
       <c r="G118" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" ht="15">
+      <c r="H118">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="15">
       <c r="A119" s="1">
         <v>887000</v>
       </c>
@@ -3171,8 +3528,11 @@
       <c r="G119" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" ht="15">
+      <c r="H119">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="15">
       <c r="A120" s="1">
         <v>427000</v>
       </c>
@@ -3194,8 +3554,11 @@
       <c r="G120" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" ht="15">
+      <c r="H120">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="15">
       <c r="A121" s="1">
         <v>193000</v>
       </c>
@@ -3217,8 +3580,11 @@
       <c r="G121" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" ht="15">
+      <c r="H121">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="15">
       <c r="A122" s="1">
         <v>690000</v>
       </c>
@@ -3240,8 +3606,11 @@
       <c r="G122" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" ht="15">
+      <c r="H122">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="15">
       <c r="A123" s="1">
         <v>1105000</v>
       </c>
@@ -3263,8 +3632,11 @@
       <c r="G123" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" ht="15">
+      <c r="H123">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" ht="15">
       <c r="A124" s="1">
         <v>808000</v>
       </c>
@@ -3286,8 +3658,11 @@
       <c r="G124" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:7" ht="15">
+      <c r="H124">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" ht="15">
       <c r="A125" s="1">
         <v>1845000</v>
       </c>
@@ -3309,8 +3684,11 @@
       <c r="G125" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" ht="15">
+      <c r="H125">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" ht="15">
       <c r="A126" s="1">
         <v>1989000</v>
       </c>
@@ -3332,8 +3710,11 @@
       <c r="G126" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" ht="15">
+      <c r="H126">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="15">
       <c r="A127" s="1">
         <v>1918000</v>
       </c>
@@ -3355,8 +3736,11 @@
       <c r="G127" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" ht="15">
+      <c r="H127">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="15">
       <c r="A128" s="1">
         <v>1283000</v>
       </c>
@@ -3378,8 +3762,11 @@
       <c r="G128" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" ht="15">
+      <c r="H128">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" ht="15">
       <c r="A129" s="1">
         <v>1020000</v>
       </c>
@@ -3401,8 +3788,11 @@
       <c r="G129" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" ht="15">
+      <c r="H129">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" ht="15">
       <c r="A130" s="1">
         <v>2051000</v>
       </c>
@@ -3424,8 +3814,11 @@
       <c r="G130" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" ht="15">
+      <c r="H130">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" ht="15">
       <c r="A131" s="1">
         <v>1172000</v>
       </c>
@@ -3447,8 +3840,11 @@
       <c r="G131" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" ht="15">
+      <c r="H131">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" ht="15">
       <c r="A132" s="1">
         <v>663000</v>
       </c>
@@ -3470,8 +3866,11 @@
       <c r="G132" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" ht="15">
+      <c r="H132">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" ht="15">
       <c r="A133" s="1">
         <v>1121000</v>
       </c>
@@ -3493,8 +3892,11 @@
       <c r="G133" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" ht="15">
+      <c r="H133">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" ht="15">
       <c r="A134" s="1">
         <v>535000</v>
       </c>
@@ -3516,8 +3918,11 @@
       <c r="G134" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" ht="15">
+      <c r="H134">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" ht="15">
       <c r="A135" s="1">
         <v>1138000</v>
       </c>
@@ -3539,8 +3944,11 @@
       <c r="G135" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" ht="15">
+      <c r="H135">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" ht="15">
       <c r="A136" s="1">
         <v>2008000</v>
       </c>
@@ -3562,8 +3970,11 @@
       <c r="G136" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" ht="15">
+      <c r="H136">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" ht="15">
       <c r="A137" s="1">
         <v>1385000</v>
       </c>
@@ -3585,8 +3996,11 @@
       <c r="G137" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="138" spans="1:7" ht="15">
+      <c r="H137">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" ht="15">
       <c r="A138" s="1">
         <v>459000</v>
       </c>
@@ -3608,8 +4022,11 @@
       <c r="G138" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="1:7" ht="15">
+      <c r="H138">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" ht="15">
       <c r="A139" s="1">
         <v>643000</v>
       </c>
@@ -3631,8 +4048,11 @@
       <c r="G139" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="140" spans="1:7" ht="15">
+      <c r="H139">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" ht="15">
       <c r="A140" s="1">
         <v>1005000</v>
       </c>
@@ -3654,8 +4074,11 @@
       <c r="G140" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" ht="15">
+      <c r="H140">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" ht="15">
       <c r="A141" s="1">
         <v>2060000</v>
       </c>
@@ -3677,8 +4100,11 @@
       <c r="G141" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" ht="15">
+      <c r="H141">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" ht="15">
       <c r="A142" s="1">
         <v>782000</v>
       </c>
@@ -3700,8 +4126,11 @@
       <c r="G142" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="143" spans="1:7" ht="15">
+      <c r="H142">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" ht="15">
       <c r="A143" s="1">
         <v>1583000</v>
       </c>
@@ -3723,8 +4152,11 @@
       <c r="G143" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:7" ht="15">
+      <c r="H143">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" ht="15">
       <c r="A144" s="1">
         <v>1762000</v>
       </c>
@@ -3746,8 +4178,11 @@
       <c r="G144" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" ht="15">
+      <c r="H144">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" ht="15">
       <c r="A145" s="1">
         <v>1265000</v>
       </c>
@@ -3769,8 +4204,11 @@
       <c r="G145" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" ht="15">
+      <c r="H145">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" ht="15">
       <c r="A146" s="1">
         <v>950000</v>
       </c>
@@ -3792,8 +4230,11 @@
       <c r="G146" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" ht="15">
+      <c r="H146">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" ht="15">
       <c r="A147" s="1">
         <v>1585000</v>
       </c>
@@ -3815,8 +4256,11 @@
       <c r="G147" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="148" spans="1:7" ht="15">
+      <c r="H147">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" ht="15">
       <c r="A148" s="1">
         <v>975000</v>
       </c>
@@ -3838,8 +4282,11 @@
       <c r="G148" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="149" spans="1:7" ht="15">
+      <c r="H148">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" ht="15">
       <c r="A149" s="1">
         <v>171000</v>
       </c>
@@ -3861,8 +4308,11 @@
       <c r="G149" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="150" spans="1:7" ht="15">
+      <c r="H149">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" ht="15">
       <c r="A150" s="1">
         <v>811000</v>
       </c>
@@ -3884,8 +4334,11 @@
       <c r="G150" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="151" spans="1:7" ht="15">
+      <c r="H150">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" ht="15">
       <c r="A151" s="1">
         <v>758000</v>
       </c>
@@ -3907,8 +4360,11 @@
       <c r="G151" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="152" spans="1:7" ht="15">
+      <c r="H151">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" ht="15">
       <c r="A152" s="1">
         <v>450000</v>
       </c>
@@ -3930,8 +4386,11 @@
       <c r="G152" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="153" spans="1:7" ht="15">
+      <c r="H152">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" ht="15">
       <c r="A153" s="1">
         <v>1514000</v>
       </c>
@@ -3953,8 +4412,11 @@
       <c r="G153" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="154" spans="1:7" ht="15">
+      <c r="H153">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" ht="15">
       <c r="A154" s="1">
         <v>784000</v>
       </c>
@@ -3976,8 +4438,11 @@
       <c r="G154" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="155" spans="1:7" ht="15">
+      <c r="H154">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" ht="15">
       <c r="A155" s="1">
         <v>1672000</v>
       </c>
@@ -3999,8 +4464,11 @@
       <c r="G155" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="156" spans="1:7" ht="15">
+      <c r="H155">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" ht="15">
       <c r="A156" s="1">
         <v>1972000</v>
       </c>
@@ -4022,8 +4490,11 @@
       <c r="G156" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="157" spans="1:7" ht="15">
+      <c r="H156">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" ht="15">
       <c r="A157" s="1">
         <v>1433000</v>
       </c>
@@ -4045,8 +4516,11 @@
       <c r="G157" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="158" spans="1:7" ht="15">
+      <c r="H157">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" ht="15">
       <c r="A158" s="1">
         <v>940000</v>
       </c>
@@ -4068,8 +4542,11 @@
       <c r="G158" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="159" spans="1:7" ht="15">
+      <c r="H158">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" ht="15">
       <c r="A159" s="1">
         <v>326000</v>
       </c>
@@ -4091,8 +4568,11 @@
       <c r="G159" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="160" spans="1:7" ht="15">
+      <c r="H159">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" ht="15">
       <c r="A160" s="1">
         <v>1374000</v>
       </c>
@@ -4114,8 +4594,11 @@
       <c r="G160" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="161" spans="1:7" ht="15">
+      <c r="H160">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" ht="15">
       <c r="A161" s="1">
         <v>1836000</v>
       </c>
@@ -4137,8 +4620,11 @@
       <c r="G161" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="162" spans="1:7" ht="15">
+      <c r="H161">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" ht="15">
       <c r="A162" s="1">
         <v>1334000</v>
       </c>
@@ -4160,8 +4646,11 @@
       <c r="G162" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="163" spans="1:7" ht="15">
+      <c r="H162">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" ht="15">
       <c r="A163" s="1">
         <v>541000</v>
       </c>
@@ -4183,8 +4672,11 @@
       <c r="G163" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="164" spans="1:7" ht="15">
+      <c r="H163">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" ht="15">
       <c r="A164" s="1">
         <v>351000</v>
       </c>
@@ -4206,8 +4698,11 @@
       <c r="G164" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="165" spans="1:7" ht="15">
+      <c r="H164">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" ht="15">
       <c r="A165" s="1">
         <v>614000</v>
       </c>
@@ -4229,8 +4724,11 @@
       <c r="G165" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="166" spans="1:7" ht="15">
+      <c r="H165">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" ht="15">
       <c r="A166" s="1">
         <v>858000</v>
       </c>
@@ -4252,8 +4750,11 @@
       <c r="G166" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="167" spans="1:7" ht="15">
+      <c r="H166">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" ht="15">
       <c r="A167" s="1">
         <v>1377000</v>
       </c>
@@ -4275,8 +4776,11 @@
       <c r="G167" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="168" spans="1:7" ht="15">
+      <c r="H167">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" ht="15">
       <c r="A168" s="1">
         <v>638000</v>
       </c>
@@ -4298,8 +4802,11 @@
       <c r="G168" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="169" spans="1:7" ht="15">
+      <c r="H168">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" ht="15">
       <c r="A169" s="1">
         <v>1882000</v>
       </c>
@@ -4321,8 +4828,11 @@
       <c r="G169" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="170" spans="1:7" ht="15">
+      <c r="H169">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" ht="15">
       <c r="A170" s="1">
         <v>1371000</v>
       </c>
@@ -4344,8 +4854,11 @@
       <c r="G170" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="171" spans="1:7" ht="15">
+      <c r="H170">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" ht="15">
       <c r="A171" s="1">
         <v>504000</v>
       </c>
@@ -4367,8 +4880,11 @@
       <c r="G171" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="172" spans="1:7" ht="15">
+      <c r="H171">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" ht="15">
       <c r="A172" s="1">
         <v>2033000</v>
       </c>
@@ -4390,8 +4906,11 @@
       <c r="G172" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="173" spans="1:7" ht="15">
+      <c r="H172">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" ht="15">
       <c r="A173" s="1">
         <v>1977000</v>
       </c>
@@ -4413,8 +4932,11 @@
       <c r="G173" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="174" spans="1:7" ht="15">
+      <c r="H173">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" ht="15">
       <c r="A174" s="1">
         <v>334000</v>
       </c>
@@ -4436,8 +4958,11 @@
       <c r="G174" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="175" spans="1:7" ht="15">
+      <c r="H174">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" ht="15">
       <c r="A175" s="1">
         <v>1263000</v>
       </c>
@@ -4459,8 +4984,11 @@
       <c r="G175" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="176" spans="1:7" ht="15">
+      <c r="H175">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" ht="15">
       <c r="A176" s="1">
         <v>1395000</v>
       </c>
@@ -4482,8 +5010,11 @@
       <c r="G176" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="177" spans="1:7" ht="15">
+      <c r="H176">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" ht="15">
       <c r="A177" s="1">
         <v>293000</v>
       </c>
@@ -4505,8 +5036,11 @@
       <c r="G177" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="178" spans="1:7" ht="15">
+      <c r="H177">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" ht="15">
       <c r="A178" s="1">
         <v>1480000</v>
       </c>
@@ -4528,8 +5062,11 @@
       <c r="G178" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="179" spans="1:7" ht="15">
+      <c r="H178">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" ht="15">
       <c r="A179" s="1">
         <v>297000</v>
       </c>
@@ -4551,8 +5088,11 @@
       <c r="G179" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="180" spans="1:7" ht="15">
+      <c r="H179">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" ht="15">
       <c r="A180" s="1">
         <v>1547000</v>
       </c>
@@ -4574,8 +5114,11 @@
       <c r="G180" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="181" spans="1:7" ht="15">
+      <c r="H180">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" ht="15">
       <c r="A181" s="1">
         <v>1279000</v>
       </c>
@@ -4597,8 +5140,11 @@
       <c r="G181" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="182" spans="1:7" ht="15">
+      <c r="H181">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" ht="15">
       <c r="A182" s="1">
         <v>1676000</v>
       </c>
@@ -4620,8 +5166,11 @@
       <c r="G182" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="183" spans="1:7" ht="15">
+      <c r="H182">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" ht="15">
       <c r="A183" s="1">
         <v>358000</v>
       </c>
@@ -4643,8 +5192,11 @@
       <c r="G183" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="184" spans="1:7" ht="15">
+      <c r="H183">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" ht="15">
       <c r="A184" s="1">
         <v>1262000</v>
       </c>
@@ -4666,8 +5218,11 @@
       <c r="G184" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="185" spans="1:7" ht="15">
+      <c r="H184">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" ht="15">
       <c r="A185" s="1">
         <v>1036000</v>
       </c>
@@ -4689,8 +5244,11 @@
       <c r="G185" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="186" spans="1:7" ht="15">
+      <c r="H185">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" ht="15">
       <c r="A186" s="1">
         <v>1094000</v>
       </c>
@@ -4712,8 +5270,11 @@
       <c r="G186" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="187" spans="1:7" ht="15">
+      <c r="H186">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" ht="15">
       <c r="A187" s="1">
         <v>732000</v>
       </c>
@@ -4735,8 +5296,11 @@
       <c r="G187" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="188" spans="1:7" ht="15">
+      <c r="H187">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" ht="15">
       <c r="A188" s="1">
         <v>1482000</v>
       </c>
@@ -4758,8 +5322,11 @@
       <c r="G188" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="189" spans="1:7" ht="15">
+      <c r="H188">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" ht="15">
       <c r="A189" s="1">
         <v>350000</v>
       </c>
@@ -4781,8 +5348,11 @@
       <c r="G189" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="190" spans="1:7" ht="15">
+      <c r="H189">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" ht="15">
       <c r="A190" s="1">
         <v>1229000</v>
       </c>
@@ -4804,8 +5374,11 @@
       <c r="G190" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="191" spans="1:7" ht="15">
+      <c r="H190">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" ht="15">
       <c r="A191" s="1">
         <v>888000</v>
       </c>
@@ -4827,8 +5400,11 @@
       <c r="G191" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="192" spans="1:7" ht="15">
+      <c r="H191">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" ht="15">
       <c r="A192" s="1">
         <v>1425000</v>
       </c>
@@ -4850,8 +5426,11 @@
       <c r="G192" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="193" spans="1:7" ht="15">
+      <c r="H192">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" ht="15">
       <c r="A193" s="1">
         <v>1740000</v>
       </c>
@@ -4873,8 +5452,11 @@
       <c r="G193" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="194" spans="1:7" ht="15">
+      <c r="H193">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" ht="15">
       <c r="A194" s="1">
         <v>1572000</v>
       </c>
@@ -4896,8 +5478,11 @@
       <c r="G194" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="195" spans="1:7" ht="15">
+      <c r="H194">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" ht="15">
       <c r="A195" s="1">
         <v>1883000</v>
       </c>
@@ -4919,8 +5504,11 @@
       <c r="G195" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="196" spans="1:7" ht="15">
+      <c r="H195">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" ht="15">
       <c r="A196" s="1">
         <v>770000</v>
       </c>
@@ -4942,8 +5530,11 @@
       <c r="G196" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="197" spans="1:7" ht="15">
+      <c r="H196">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" ht="15">
       <c r="A197" s="1">
         <v>974000</v>
       </c>
@@ -4965,8 +5556,11 @@
       <c r="G197" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="198" spans="1:7" ht="15">
+      <c r="H197">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" ht="15">
       <c r="A198" s="1">
         <v>583000</v>
       </c>
@@ -4988,8 +5582,11 @@
       <c r="G198" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="199" spans="1:7" ht="15">
+      <c r="H198">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" ht="15">
       <c r="A199" s="1">
         <v>1550000</v>
       </c>
@@ -5011,8 +5608,11 @@
       <c r="G199" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="200" spans="1:7" ht="15">
+      <c r="H199">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" ht="15">
       <c r="A200" s="1">
         <v>548000</v>
       </c>
@@ -5034,8 +5634,11 @@
       <c r="G200" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="201" spans="1:7" ht="15">
+      <c r="H200">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" ht="15">
       <c r="A201" s="1">
         <v>1804000</v>
       </c>
@@ -5057,8 +5660,11 @@
       <c r="G201" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="202" spans="1:7" ht="15">
+      <c r="H201">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" ht="15">
       <c r="A202" s="1">
         <v>751000</v>
       </c>
@@ -5080,8 +5686,11 @@
       <c r="G202" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="203" spans="1:7" ht="15">
+      <c r="H202">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" ht="15">
       <c r="A203" s="1">
         <v>595000</v>
       </c>
@@ -5103,8 +5712,11 @@
       <c r="G203" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="204" spans="1:7" ht="15">
+      <c r="H203">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" ht="15">
       <c r="A204" s="1">
         <v>1023000</v>
       </c>
@@ -5126,8 +5738,11 @@
       <c r="G204" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="205" spans="1:7" ht="15">
+      <c r="H204">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" ht="15">
       <c r="A205" s="1">
         <v>1092000</v>
       </c>
@@ -5149,8 +5764,11 @@
       <c r="G205" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="206" spans="1:7" ht="15">
+      <c r="H205">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" ht="15">
       <c r="A206" s="1">
         <v>1263000</v>
       </c>
@@ -5172,8 +5790,11 @@
       <c r="G206" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="207" spans="1:7" ht="15">
+      <c r="H206">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" ht="15">
       <c r="A207" s="1">
         <v>540000</v>
       </c>
@@ -5195,8 +5816,11 @@
       <c r="G207" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="208" spans="1:7" ht="15">
+      <c r="H207">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" ht="15">
       <c r="A208" s="1">
         <v>234000</v>
       </c>
@@ -5218,8 +5842,11 @@
       <c r="G208" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="209" spans="1:7" ht="15">
+      <c r="H208">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" ht="15">
       <c r="A209" s="1">
         <v>1526000</v>
       </c>
@@ -5241,8 +5868,11 @@
       <c r="G209" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="210" spans="1:7" ht="15">
+      <c r="H209">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" ht="15">
       <c r="A210" s="1">
         <v>845000</v>
       </c>
@@ -5264,8 +5894,11 @@
       <c r="G210" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="211" spans="1:7" ht="15">
+      <c r="H210">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" ht="15">
       <c r="A211" s="1">
         <v>305000</v>
       </c>
@@ -5287,8 +5920,11 @@
       <c r="G211" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="212" spans="1:7" ht="15">
+      <c r="H211">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" ht="15">
       <c r="A212" s="1">
         <v>478000</v>
       </c>
@@ -5310,8 +5946,11 @@
       <c r="G212" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="213" spans="1:7" ht="15">
+      <c r="H212">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" ht="15">
       <c r="A213" s="1">
         <v>1802000</v>
       </c>
@@ -5333,8 +5972,11 @@
       <c r="G213" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="214" spans="1:7" ht="15">
+      <c r="H213">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" ht="15">
       <c r="A214" s="1">
         <v>1582000</v>
       </c>
@@ -5356,8 +5998,11 @@
       <c r="G214" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="215" spans="1:7" ht="15">
+      <c r="H214">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" ht="15">
       <c r="A215" s="1">
         <v>329000</v>
       </c>
@@ -5379,8 +6024,11 @@
       <c r="G215" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="216" spans="1:7" ht="15">
+      <c r="H215">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" ht="15">
       <c r="A216" s="1">
         <v>779000</v>
       </c>
@@ -5402,8 +6050,11 @@
       <c r="G216" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="217" spans="1:7" ht="15">
+      <c r="H216">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" ht="15">
       <c r="A217" s="1">
         <v>1036000</v>
       </c>
@@ -5425,8 +6076,11 @@
       <c r="G217" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="218" spans="1:7" ht="15">
+      <c r="H217">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" ht="15">
       <c r="A218" s="1">
         <v>1109000</v>
       </c>
@@ -5448,8 +6102,11 @@
       <c r="G218" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="219" spans="1:7" ht="15">
+      <c r="H218">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" ht="15">
       <c r="A219" s="1">
         <v>1532000</v>
       </c>
@@ -5471,8 +6128,11 @@
       <c r="G219" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="220" spans="1:7" ht="15">
+      <c r="H219">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" ht="15">
       <c r="A220" s="1">
         <v>1393000</v>
       </c>
@@ -5494,8 +6154,11 @@
       <c r="G220" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="221" spans="1:7" ht="15">
+      <c r="H220">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" ht="15">
       <c r="A221" s="1">
         <v>1693000</v>
       </c>
@@ -5517,8 +6180,11 @@
       <c r="G221" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="222" spans="1:7" ht="15">
+      <c r="H221">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" ht="15">
       <c r="A222" s="1">
         <v>401000</v>
       </c>
@@ -5540,8 +6206,11 @@
       <c r="G222" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="223" spans="1:7" ht="15">
+      <c r="H222">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" ht="15">
       <c r="A223" s="1">
         <v>1416000</v>
       </c>
@@ -5563,8 +6232,11 @@
       <c r="G223" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="224" spans="1:7" ht="15">
+      <c r="H223">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" ht="15">
       <c r="A224" s="1">
         <v>1844000</v>
       </c>
@@ -5586,8 +6258,11 @@
       <c r="G224" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="225" spans="1:7" ht="15">
+      <c r="H224">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" ht="15">
       <c r="A225" s="1">
         <v>870000</v>
       </c>
@@ -5609,8 +6284,11 @@
       <c r="G225" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="226" spans="1:7" ht="15">
+      <c r="H225">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" ht="15">
       <c r="A226" s="1">
         <v>1408000</v>
       </c>
@@ -5632,8 +6310,11 @@
       <c r="G226" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="227" spans="1:7" ht="15">
+      <c r="H226">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" ht="15">
       <c r="A227" s="1">
         <v>1865000</v>
       </c>
@@ -5655,8 +6336,11 @@
       <c r="G227" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="228" spans="1:7" ht="15">
+      <c r="H227">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" ht="15">
       <c r="A228" s="1">
         <v>718000</v>
       </c>
@@ -5678,8 +6362,11 @@
       <c r="G228" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="229" spans="1:7" ht="15">
+      <c r="H228">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" ht="15">
       <c r="A229" s="1">
         <v>1249000</v>
       </c>
@@ -5701,8 +6388,11 @@
       <c r="G229" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="230" spans="1:7" ht="15">
+      <c r="H229">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" ht="15">
       <c r="A230" s="1">
         <v>1289000</v>
       </c>
@@ -5724,8 +6414,11 @@
       <c r="G230" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="231" spans="1:7" ht="15">
+      <c r="H230">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" ht="15">
       <c r="A231" s="1">
         <v>1177000</v>
       </c>
@@ -5747,8 +6440,11 @@
       <c r="G231" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="232" spans="1:7" ht="15">
+      <c r="H231">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8" ht="15">
       <c r="A232" s="1">
         <v>948000</v>
       </c>
@@ -5770,8 +6466,11 @@
       <c r="G232" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="233" spans="1:7" ht="15">
+      <c r="H232">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" ht="15">
       <c r="A233" s="1">
         <v>1433000</v>
       </c>
@@ -5793,8 +6492,11 @@
       <c r="G233" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="234" spans="1:7" ht="15">
+      <c r="H233">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" ht="15">
       <c r="A234" s="1">
         <v>515000</v>
       </c>
@@ -5816,8 +6518,11 @@
       <c r="G234" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="235" spans="1:7" ht="15">
+      <c r="H234">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" ht="15">
       <c r="A235" s="1">
         <v>1958000</v>
       </c>
@@ -5839,8 +6544,11 @@
       <c r="G235" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="236" spans="1:7" ht="15">
+      <c r="H235">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8" ht="15">
       <c r="A236" s="1">
         <v>1775000</v>
       </c>
@@ -5862,8 +6570,11 @@
       <c r="G236" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="237" spans="1:7" ht="15">
+      <c r="H236">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8" ht="15">
       <c r="A237" s="1">
         <v>479000</v>
       </c>
@@ -5885,8 +6596,11 @@
       <c r="G237" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="238" spans="1:7" ht="15">
+      <c r="H237">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8" ht="15">
       <c r="A238" s="1">
         <v>620000</v>
       </c>
@@ -5908,8 +6622,11 @@
       <c r="G238" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="239" spans="1:7" ht="15">
+      <c r="H238">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8" ht="15">
       <c r="A239" s="1">
         <v>1208000</v>
       </c>
@@ -5931,8 +6648,11 @@
       <c r="G239" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="240" spans="1:7" ht="15">
+      <c r="H239">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8" ht="15">
       <c r="A240" s="1">
         <v>1170000</v>
       </c>
@@ -5954,8 +6674,11 @@
       <c r="G240" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="241" spans="1:7" ht="15">
+      <c r="H240">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8" ht="15">
       <c r="A241" s="1">
         <v>1565000</v>
       </c>
@@ -5977,8 +6700,11 @@
       <c r="G241" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="242" spans="1:7" ht="15">
+      <c r="H241">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8" ht="15">
       <c r="A242" s="1">
         <v>874000</v>
       </c>
@@ -6000,8 +6726,11 @@
       <c r="G242" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="243" spans="1:7" ht="15">
+      <c r="H242">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8" ht="15">
       <c r="A243" s="1">
         <v>820000</v>
       </c>
@@ -6023,8 +6752,11 @@
       <c r="G243" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="244" spans="1:7" ht="15">
+      <c r="H243">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" ht="15">
       <c r="A244" s="1">
         <v>1208000</v>
       </c>
@@ -6046,8 +6778,11 @@
       <c r="G244" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="245" spans="1:7" ht="15">
+      <c r="H244">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8" ht="15">
       <c r="A245" s="1">
         <v>2001000</v>
       </c>
@@ -6069,8 +6804,11 @@
       <c r="G245" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="246" spans="1:7" ht="15">
+      <c r="H245">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" ht="15">
       <c r="A246" s="1">
         <v>1889000</v>
       </c>
@@ -6092,8 +6830,11 @@
       <c r="G246" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="247" spans="1:7" ht="15">
+      <c r="H246">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" ht="15">
       <c r="A247" s="1">
         <v>1420000</v>
       </c>
@@ -6115,8 +6856,11 @@
       <c r="G247" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="248" spans="1:7" ht="15">
+      <c r="H247">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" ht="15">
       <c r="A248" s="1">
         <v>1140000</v>
       </c>
@@ -6138,8 +6882,11 @@
       <c r="G248" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="249" spans="1:7" ht="15">
+      <c r="H248">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8" ht="15">
       <c r="A249" s="1">
         <v>1751000</v>
       </c>
@@ -6161,8 +6908,11 @@
       <c r="G249" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="250" spans="1:7" ht="15">
+      <c r="H249">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" ht="15">
       <c r="A250" s="1">
         <v>1048000</v>
       </c>
@@ -6184,8 +6934,11 @@
       <c r="G250" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="251" spans="1:7" ht="15">
+      <c r="H250">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" ht="15">
       <c r="A251" s="1">
         <v>891000</v>
       </c>
@@ -6207,8 +6960,11 @@
       <c r="G251" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="252" spans="1:7" ht="15">
+      <c r="H251">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" ht="15">
       <c r="A252" s="1">
         <v>1993000</v>
       </c>
@@ -6230,8 +6986,11 @@
       <c r="G252" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="253" spans="1:7" ht="15">
+      <c r="H252">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" ht="15">
       <c r="A253" s="1">
         <v>1767000</v>
       </c>
@@ -6253,8 +7012,11 @@
       <c r="G253" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="254" spans="1:7" ht="15">
+      <c r="H253">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" ht="15">
       <c r="A254" s="1">
         <v>1411000</v>
       </c>
@@ -6276,8 +7038,11 @@
       <c r="G254" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="255" spans="1:7" ht="15">
+      <c r="H254">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" ht="15">
       <c r="A255" s="1">
         <v>794000</v>
       </c>
@@ -6299,8 +7064,11 @@
       <c r="G255" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="256" spans="1:7" ht="15">
+      <c r="H255">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" ht="15">
       <c r="A256" s="1">
         <v>346000</v>
       </c>
@@ -6322,8 +7090,11 @@
       <c r="G256" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="257" spans="1:7" ht="15">
+      <c r="H256">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8" ht="15">
       <c r="A257" s="1">
         <v>209000</v>
       </c>
@@ -6345,8 +7116,11 @@
       <c r="G257" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="258" spans="1:7" ht="15">
+      <c r="H257">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8" ht="15">
       <c r="A258" s="1">
         <v>1562000</v>
       </c>
@@ -6367,6 +7141,9 @@
       </c>
       <c r="G258" s="1">
         <v>1</v>
+      </c>
+      <c r="H258">
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -6375,15 +7152,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100C0AE222F8A32CD4684F55E4BA37FAF03" ma:contentTypeVersion="13" ma:contentTypeDescription="Utwórz nowy dokument." ma:contentTypeScope="" ma:versionID="c65b25c046bc2806eea7e0f48b1f7a85">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="85748aa4-f3fa-451f-976a-f4f3da3c6bcd" xmlns:ns4="dd79dbaa-7478-4d49-9bb6-590314044112" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9b42e451194490ccd2eab0876ab5e7f7" ns3:_="" ns4:_="">
     <xsd:import namespace="85748aa4-f3fa-451f-976a-f4f3da3c6bcd"/>
@@ -6606,6 +7374,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -6615,11 +7392,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7101A2A-67D5-4A8E-A893-1841D13A8222}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9BA115B-AE8A-4EB5-8515-53524BEEE0DF}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9BA115B-AE8A-4EB5-8515-53524BEEE0DF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7101A2A-67D5-4A8E-A893-1841D13A8222}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>